<commit_message>
checking if the primary key is unique
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6030"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Nom</t>
   </si>
@@ -72,6 +72,27 @@
   </si>
   <si>
     <t>mohmed@gmail.com</t>
+  </si>
+  <si>
+    <t>Numero</t>
+  </si>
+  <si>
+    <t>dari</t>
+  </si>
+  <si>
+    <t>hala</t>
+  </si>
+  <si>
+    <t>haja@gmail.com</t>
+  </si>
+  <si>
+    <t>gg</t>
+  </si>
+  <si>
+    <t>dfd</t>
+  </si>
+  <si>
+    <t>gg@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -400,20 +421,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="7.85546875" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" customWidth="1"/>
     <col min="5" max="5" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -427,7 +452,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>123</v>
+      </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
@@ -441,7 +469,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>456</v>
+      </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -455,7 +486,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>789</v>
+      </c>
       <c r="B4" t="s">
         <v>13</v>
       </c>
@@ -469,7 +503,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>21</v>
+      </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
@@ -481,6 +518,40 @@
       </c>
       <c r="E5" s="1" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6">
+        <v>123456789</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>123</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7">
+        <v>1233</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -489,6 +560,8 @@
     <hyperlink ref="E5" r:id="rId2"/>
     <hyperlink ref="E2" r:id="rId3"/>
     <hyperlink ref="E4" r:id="rId4"/>
+    <hyperlink ref="E6" r:id="rId5"/>
+    <hyperlink ref="E7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>